<commit_message>
Add code and check figure
</commit_message>
<xml_diff>
--- a/solow/basicsolow.xlsx
+++ b/solow/basicsolow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dietz/Dropbox/Project/StudyGuide/solow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C180982-5A8E-A74D-9C38-93EFBF7E1FD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2657DA4A-807D-7A47-9F55-0940E4649233}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -117,6 +120,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -4335,8 +4339,8 @@
   </sheetPr>
   <dimension ref="A1:K1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>